<commit_message>
Renamed pop_age_pyramid to age-gender_pyramid for .sql, .xlsx, and .csv, as well as changing database view name
</commit_message>
<xml_diff>
--- a/reports/age-gender_pyramid.xlsx
+++ b/reports/age-gender_pyramid.xlsx
@@ -9,9 +9,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="pop_age_pyramid" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="pop_age_pyramid_1" localSheetId="0">Sheet1!$A$1:$S$11</definedName>
@@ -28,7 +25,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="pop_age_pyramid.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:Charles:Documents:hea_baselines:south_africa:baselines_surveys:2016_lp_mp:reports:pop_age_pyramid.csv" tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:Charles:Documents:hea_baselines:south_africa:baselines_surveys:2016_lp_mp:reports:pop_age_pyramid.csv" tab="0" comma="1">
       <textFields count="19">
         <textField/>
         <textField/>
@@ -564,11 +561,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="1808386216"/>
-        <c:axId val="1808354104"/>
+        <c:axId val="-2035865288"/>
+        <c:axId val="1793203976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1808386216"/>
+        <c:axId val="-2035865288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -597,7 +594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1808354104"/>
+        <c:crossAx val="1793203976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -605,7 +602,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1808354104"/>
+        <c:axId val="1793203976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -646,7 +643,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1808386216"/>
+        <c:crossAx val="-2035865288"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.02"/>
@@ -1074,11 +1071,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="2103165752"/>
-        <c:axId val="1809638984"/>
+        <c:axId val="1822356264"/>
+        <c:axId val="1821281112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2103165752"/>
+        <c:axId val="1822356264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,7 +1104,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1809638984"/>
+        <c:crossAx val="1821281112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1115,7 +1112,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1809638984"/>
+        <c:axId val="1821281112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -1156,7 +1153,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103165752"/>
+        <c:crossAx val="1822356264"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.02"/>
@@ -1584,11 +1581,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="1810859336"/>
-        <c:axId val="1793264136"/>
+        <c:axId val="1822005496"/>
+        <c:axId val="2104047560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1810859336"/>
+        <c:axId val="1822005496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,7 +1614,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1793264136"/>
+        <c:crossAx val="2104047560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1625,7 +1622,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1793264136"/>
+        <c:axId val="2104047560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -1666,7 +1663,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1810859336"/>
+        <c:crossAx val="1822005496"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.02"/>
@@ -2094,11 +2091,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="1810170840"/>
-        <c:axId val="1810474312"/>
+        <c:axId val="-2053039368"/>
+        <c:axId val="1822810712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1810170840"/>
+        <c:axId val="-2053039368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2127,7 +2124,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1810474312"/>
+        <c:crossAx val="1822810712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2135,7 +2132,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1810474312"/>
+        <c:axId val="1822810712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -2176,7 +2173,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1810170840"/>
+        <c:crossAx val="-2053039368"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.02"/>
@@ -2604,11 +2601,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="1794380712"/>
-        <c:axId val="1790080888"/>
+        <c:axId val="1786786280"/>
+        <c:axId val="1809179928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1794380712"/>
+        <c:axId val="1786786280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2637,7 +2634,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1790080888"/>
+        <c:crossAx val="1809179928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2645,7 +2642,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1790080888"/>
+        <c:axId val="1809179928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -2686,7 +2683,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1794380712"/>
+        <c:crossAx val="1786786280"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.02"/>
@@ -2918,196 +2915,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="data"/>
-      <sheetName val="result"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="C1" t="str">
-            <v>0 - 4</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>5 - 9</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>10 - 14</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>15 - 19</v>
-          </cell>
-          <cell r="G1" t="str">
-            <v>20 - 24</v>
-          </cell>
-          <cell r="H1" t="str">
-            <v>25 - 29</v>
-          </cell>
-          <cell r="I1" t="str">
-            <v>30 - 34</v>
-          </cell>
-          <cell r="J1" t="str">
-            <v>35 - 39</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v>40 - 44</v>
-          </cell>
-          <cell r="L1" t="str">
-            <v>45 - 49</v>
-          </cell>
-          <cell r="M1" t="str">
-            <v>50 - 54</v>
-          </cell>
-          <cell r="N1" t="str">
-            <v>55 - 59</v>
-          </cell>
-          <cell r="O1" t="str">
-            <v>60 - 64</v>
-          </cell>
-          <cell r="P1" t="str">
-            <v>65 - 69</v>
-          </cell>
-          <cell r="Q1" t="str">
-            <v>70 - 74</v>
-          </cell>
-          <cell r="R1" t="str">
-            <v>75 - 79</v>
-          </cell>
-          <cell r="S1" t="str">
-            <v>80 - 84</v>
-          </cell>
-          <cell r="T1" t="str">
-            <v>85+</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23" t="str">
-            <v>female, all LZs</v>
-          </cell>
-          <cell r="C23">
-            <v>6.9900000000000004E-2</v>
-          </cell>
-          <cell r="D23">
-            <v>6.1499999999999999E-2</v>
-          </cell>
-          <cell r="E23">
-            <v>5.9900000000000002E-2</v>
-          </cell>
-          <cell r="F23">
-            <v>6.3299999999999995E-2</v>
-          </cell>
-          <cell r="G23">
-            <v>5.2299999999999999E-2</v>
-          </cell>
-          <cell r="H23">
-            <v>4.3099999999999999E-2</v>
-          </cell>
-          <cell r="I23">
-            <v>3.09E-2</v>
-          </cell>
-          <cell r="J23">
-            <v>2.5100000000000001E-2</v>
-          </cell>
-          <cell r="K23">
-            <v>2.2200000000000001E-2</v>
-          </cell>
-          <cell r="L23">
-            <v>2.2800000000000001E-2</v>
-          </cell>
-          <cell r="M23">
-            <v>1.9699999999999999E-2</v>
-          </cell>
-          <cell r="N23">
-            <v>1.7100000000000001E-2</v>
-          </cell>
-          <cell r="O23">
-            <v>1.52E-2</v>
-          </cell>
-          <cell r="P23">
-            <v>0.01</v>
-          </cell>
-          <cell r="Q23">
-            <v>9.1000000000000004E-3</v>
-          </cell>
-          <cell r="R23">
-            <v>6.1999999999999998E-3</v>
-          </cell>
-          <cell r="S23">
-            <v>5.1999999999999998E-3</v>
-          </cell>
-          <cell r="T23">
-            <v>3.5999999999999999E-3</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24" t="str">
-            <v>male, all LZs</v>
-          </cell>
-          <cell r="C24">
-            <v>-7.0499999999999993E-2</v>
-          </cell>
-          <cell r="D24">
-            <v>-6.2799999999999995E-2</v>
-          </cell>
-          <cell r="E24">
-            <v>-6.3399999999999998E-2</v>
-          </cell>
-          <cell r="F24">
-            <v>-6.3700000000000007E-2</v>
-          </cell>
-          <cell r="G24">
-            <v>-4.5699999999999998E-2</v>
-          </cell>
-          <cell r="H24">
-            <v>-3.39E-2</v>
-          </cell>
-          <cell r="I24">
-            <v>-2.3800000000000002E-2</v>
-          </cell>
-          <cell r="J24">
-            <v>-0.02</v>
-          </cell>
-          <cell r="K24">
-            <v>-1.52E-2</v>
-          </cell>
-          <cell r="L24">
-            <v>-1.4200000000000001E-2</v>
-          </cell>
-          <cell r="M24">
-            <v>-1.2500000000000001E-2</v>
-          </cell>
-          <cell r="N24">
-            <v>-1.14E-2</v>
-          </cell>
-          <cell r="O24">
-            <v>-9.7000000000000003E-3</v>
-          </cell>
-          <cell r="P24">
-            <v>-5.4999999999999997E-3</v>
-          </cell>
-          <cell r="Q24">
-            <v>-4.1000000000000003E-3</v>
-          </cell>
-          <cell r="R24">
-            <v>-2E-3</v>
-          </cell>
-          <cell r="S24">
-            <v>-1.5E-3</v>
-          </cell>
-          <cell r="T24">
-            <v>-1.1999999999999999E-3</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3438,7 +3245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>

</xml_diff>